<commit_message>
concluída a config em todos os equipamentos
</commit_message>
<xml_diff>
--- a/Azure CLI.xlsx
+++ b/Azure CLI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willian.lima\Documents\GitHub\AnotacoesCloud-AZ104\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willian.lima\repositorios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4563BB98-48F6-48AF-A361-F8DEED6C5855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565ABE87-1E54-435B-8701-734AD5E1D3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{67543718-3FB2-4D8C-AB3B-EE72DB600CBB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{67543718-3FB2-4D8C-AB3B-EE72DB600CBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Comando</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>Listar todos os tamanhos disponíveis de VM em uma localização</t>
-  </si>
-  <si>
-    <t>teste</t>
   </si>
 </sst>
 </file>
@@ -521,18 +518,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D79F9FF-3C83-474C-96E9-0B7F79969C03}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="72.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="72.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -540,7 +537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -548,7 +545,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -556,7 +553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -564,7 +561,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -572,7 +569,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -580,7 +577,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -588,7 +585,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -596,7 +593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -604,7 +601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -612,7 +609,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -620,7 +617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -628,7 +625,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -636,7 +633,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -644,7 +641,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -652,7 +649,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -660,7 +657,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -668,7 +665,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -676,17 +673,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>